<commit_message>
JM is done with regression test
</commit_message>
<xml_diff>
--- a/DataExtraction1/baseline-hysys.xlsx
+++ b/DataExtraction1/baseline-hysys.xlsx
@@ -1,38 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gutierrj\source\repos\data_transfer\DataExtraction1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gutierrj\source\repos\datatransfer-ProII\DataExtraction1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1711A857-A412-42D6-9524-06328640422A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C4945FE-90EE-4928-870C-92E475E293C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{74D46F0D-D033-4CA4-8C2F-97A0182A711B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="19" xr2:uid="{74D46F0D-D033-4CA4-8C2F-97A0182A711B}"/>
   </bookViews>
   <sheets>
     <sheet name="Pump &amp; Pump Curves" sheetId="1" r:id="rId1"/>
-    <sheet name="Rigorous FireHeater" sheetId="2" r:id="rId2"/>
-    <sheet name="HeaterCooler" sheetId="19" r:id="rId3"/>
-    <sheet name="Multimapping-HXHotSide" sheetId="3" r:id="rId4"/>
-    <sheet name="Multimapping-HXColdSide" sheetId="4" r:id="rId5"/>
-    <sheet name="Separator" sheetId="20" r:id="rId6"/>
-    <sheet name="Valves" sheetId="5" r:id="rId7"/>
-    <sheet name="SimpleShell&amp;TubeHE" sheetId="6" r:id="rId8"/>
-    <sheet name="RigorousShell&amp;TubeHE" sheetId="7" r:id="rId9"/>
-    <sheet name="RigorousAirCooledHexchanger" sheetId="8" r:id="rId10"/>
-    <sheet name="HeatCurvesHot" sheetId="9" r:id="rId11"/>
-    <sheet name="HeatCurvesCold" sheetId="10" r:id="rId12"/>
-    <sheet name="Compressor &amp; Compressor Curves" sheetId="11" r:id="rId13"/>
-    <sheet name="MCompressor" sheetId="12" r:id="rId14"/>
-    <sheet name="Expander" sheetId="13" r:id="rId15"/>
-    <sheet name="Streams" sheetId="14" r:id="rId16"/>
-    <sheet name="Vessels" sheetId="15" r:id="rId17"/>
-    <sheet name="Utility" sheetId="16" r:id="rId18"/>
-    <sheet name="ColumnMainTS" sheetId="17" r:id="rId19"/>
-    <sheet name="ColumnTS1" sheetId="18" r:id="rId20"/>
+    <sheet name="FireHeater" sheetId="2" r:id="rId2"/>
+    <sheet name="Multimapping-HXHotSide" sheetId="3" r:id="rId3"/>
+    <sheet name="Multimapping-HXColdSide" sheetId="4" r:id="rId4"/>
+    <sheet name="Separator" sheetId="20" r:id="rId5"/>
+    <sheet name="Valves" sheetId="5" r:id="rId6"/>
+    <sheet name="SimpleShell&amp;TubeHE" sheetId="6" r:id="rId7"/>
+    <sheet name="RigorousShell&amp;TubeHE" sheetId="7" r:id="rId8"/>
+    <sheet name="RigorousAirCooledHexchanger" sheetId="8" r:id="rId9"/>
+    <sheet name="HeatCurvesHot" sheetId="9" r:id="rId10"/>
+    <sheet name="HeatCurvesCold" sheetId="10" r:id="rId11"/>
+    <sheet name="Compressor &amp; Compressor Curves" sheetId="11" r:id="rId12"/>
+    <sheet name="Expander" sheetId="13" r:id="rId13"/>
+    <sheet name="Streams" sheetId="14" r:id="rId14"/>
+    <sheet name="Vessels" sheetId="15" r:id="rId15"/>
+    <sheet name="Utility" sheetId="16" r:id="rId16"/>
+    <sheet name="MCompressor" sheetId="12" r:id="rId17"/>
+    <sheet name="ColumnMainTS" sheetId="17" r:id="rId18"/>
+    <sheet name="ColumnTS1" sheetId="18" r:id="rId19"/>
+    <sheet name="HeaterCooler" sheetId="19" r:id="rId20"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -2354,7 +2354,7 @@
   <dimension ref="A1:D44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2977,1071 +2977,6 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFDE4E1-59B7-4973-8CE1-C8EF435EF1EA}">
-  <dimension ref="A1:D83"/>
-  <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="21.5703125" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="14.140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>360</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>361</v>
-      </c>
-      <c r="C2">
-        <v>2.3103881337999899</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>360</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="C3">
-        <v>5.4722559999999998</v>
-      </c>
-      <c r="D3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>360</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C4">
-        <v>298.14999999999998</v>
-      </c>
-      <c r="D4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>360</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C5">
-        <v>475.92910262650202</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>360</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>365</v>
-      </c>
-      <c r="C6">
-        <v>4.62077626759997</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>360</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>366</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>360</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>367</v>
-      </c>
-      <c r="C8">
-        <v>5.4796446382057002</v>
-      </c>
-      <c r="D8" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>360</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>360</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="C10">
-        <v>0.60960000000000003</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>360</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>360</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="C12">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>360</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C13">
-        <v>5.7149999999999999E-2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>360</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>373</v>
-      </c>
-      <c r="C14">
-        <v>2.7990799999999999E-4</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>360</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>374</v>
-      </c>
-      <c r="C15" t="s">
-        <v>375</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>360</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>376</v>
-      </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>360</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="D17" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>360</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>378</v>
-      </c>
-      <c r="C18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>360</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>360</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>380</v>
-      </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>360</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>381</v>
-      </c>
-      <c r="C21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>360</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>382</v>
-      </c>
-      <c r="C22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>360</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>383</v>
-      </c>
-      <c r="C23">
-        <v>987095.20799758995</v>
-      </c>
-      <c r="D23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>360</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>384</v>
-      </c>
-      <c r="C24">
-        <v>274.77419665194498</v>
-      </c>
-      <c r="D24" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>360</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>385</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>360</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="C26">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>360</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>387</v>
-      </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>360</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="C28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>360</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>389</v>
-      </c>
-      <c r="C29">
-        <v>0.1463294</v>
-      </c>
-      <c r="D29" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>360</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="C30">
-        <v>0.1222502</v>
-      </c>
-      <c r="D30" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>360</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="C31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>360</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>392</v>
-      </c>
-      <c r="C32">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>360</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="C33">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>360</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="D34" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>360</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>396</v>
-      </c>
-      <c r="C35">
-        <v>128.72530222576</v>
-      </c>
-      <c r="D35" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>360</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>397</v>
-      </c>
-      <c r="C36">
-        <v>655.58755669238701</v>
-      </c>
-      <c r="D36" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>360</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>398</v>
-      </c>
-      <c r="C37">
-        <v>655.58755669238701</v>
-      </c>
-      <c r="D37" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>360</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>399</v>
-      </c>
-      <c r="C38">
-        <v>27.907387108739801</v>
-      </c>
-      <c r="D38" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>360</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>400</v>
-      </c>
-      <c r="C39">
-        <v>2.600006</v>
-      </c>
-      <c r="D39" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>360</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C40">
-        <v>31.472630310058602</v>
-      </c>
-      <c r="D40" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>360</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="D41" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>360</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>403</v>
-      </c>
-      <c r="D42" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>360</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>404</v>
-      </c>
-      <c r="D43" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>360</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>405</v>
-      </c>
-      <c r="D44" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>360</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="D45" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>360</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="D46" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>360</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="D47" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>360</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="D48" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>360</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>338</v>
-      </c>
-      <c r="C49">
-        <v>699.81666666666695</v>
-      </c>
-      <c r="D49" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>360</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>410</v>
-      </c>
-      <c r="C50">
-        <v>18.779133793301298</v>
-      </c>
-      <c r="D50" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>360</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="C51">
-        <v>5.0399669378168896</v>
-      </c>
-      <c r="D51" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>360</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>412</v>
-      </c>
-      <c r="C52">
-        <v>3362.68548838072</v>
-      </c>
-      <c r="D52" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>360</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="C53">
-        <v>8.2194160102302904E-2</v>
-      </c>
-      <c r="D53" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>360</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>414</v>
-      </c>
-      <c r="C54" s="3">
-        <v>2.1559459677269801E-5</v>
-      </c>
-      <c r="D54" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>360</v>
-      </c>
-      <c r="B55" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="D55" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>360</v>
-      </c>
-      <c r="B56" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="C56">
-        <v>30</v>
-      </c>
-      <c r="D56" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>360</v>
-      </c>
-      <c r="B57" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C57">
-        <v>2.000006</v>
-      </c>
-      <c r="D57" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>360</v>
-      </c>
-      <c r="B58" s="1" t="s">
-        <v>417</v>
-      </c>
-      <c r="C58">
-        <v>5.1960779999999998E-2</v>
-      </c>
-      <c r="D58" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>360</v>
-      </c>
-      <c r="B59" s="1" t="s">
-        <v>418</v>
-      </c>
-      <c r="C59" t="s">
-        <v>419</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>360</v>
-      </c>
-      <c r="B60" s="1" t="s">
-        <v>420</v>
-      </c>
-      <c r="C60">
-        <v>1.6509999999999999E-3</v>
-      </c>
-      <c r="D60" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>360</v>
-      </c>
-      <c r="B61" s="1" t="s">
-        <v>421</v>
-      </c>
-      <c r="C61">
-        <v>2.5399999999999999E-2</v>
-      </c>
-      <c r="D61" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>360</v>
-      </c>
-      <c r="B62" s="1" t="s">
-        <v>422</v>
-      </c>
-      <c r="D62" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>360</v>
-      </c>
-      <c r="B63" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="D63" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>360</v>
-      </c>
-      <c r="B64" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="D64" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>360</v>
-      </c>
-      <c r="B65" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="D65" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>360</v>
-      </c>
-      <c r="B66" s="1" t="s">
-        <v>426</v>
-      </c>
-      <c r="D66" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>360</v>
-      </c>
-      <c r="B67" s="1" t="s">
-        <v>427</v>
-      </c>
-      <c r="D67" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>360</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>428</v>
-      </c>
-      <c r="D68" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>360</v>
-      </c>
-      <c r="B69" s="1" t="s">
-        <v>429</v>
-      </c>
-      <c r="D69" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>360</v>
-      </c>
-      <c r="B70" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="C70">
-        <v>639.87495207500899</v>
-      </c>
-      <c r="D70" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>360</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>430</v>
-      </c>
-      <c r="C71">
-        <v>20.610095210760001</v>
-      </c>
-      <c r="D71" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>360</v>
-      </c>
-      <c r="B72" s="1" t="s">
-        <v>431</v>
-      </c>
-      <c r="C72">
-        <v>5.0399669378168896</v>
-      </c>
-      <c r="D72" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>360</v>
-      </c>
-      <c r="B73" s="1" t="s">
-        <v>432</v>
-      </c>
-      <c r="C73">
-        <v>31.472630310058602</v>
-      </c>
-      <c r="D73" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>360</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C74">
-        <v>3172.2168225098299</v>
-      </c>
-      <c r="D74" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>360</v>
-      </c>
-      <c r="B75" s="1" t="s">
-        <v>434</v>
-      </c>
-      <c r="C75">
-        <v>7.2597136537635498E-2</v>
-      </c>
-      <c r="D75" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>360</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>435</v>
-      </c>
-      <c r="C76" s="3">
-        <v>2.0231390664874999E-5</v>
-      </c>
-      <c r="D76" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>360</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>436</v>
-      </c>
-      <c r="D77" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>360</v>
-      </c>
-      <c r="B78" s="1" t="s">
-        <v>437</v>
-      </c>
-      <c r="C78">
-        <v>44473.795433876803</v>
-      </c>
-      <c r="D78" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>360</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>438</v>
-      </c>
-      <c r="C79">
-        <v>14698.051332810899</v>
-      </c>
-      <c r="D79" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>360</v>
-      </c>
-      <c r="B80" s="1" t="s">
-        <v>439</v>
-      </c>
-      <c r="C80">
-        <v>3447379.5433876798</v>
-      </c>
-      <c r="D80" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>360</v>
-      </c>
-      <c r="B81" s="1" t="s">
-        <v>440</v>
-      </c>
-      <c r="C81">
-        <v>379191.81346832501</v>
-      </c>
-      <c r="D81" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>360</v>
-      </c>
-      <c r="B82" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="C82">
-        <v>5.0399669378168896</v>
-      </c>
-      <c r="D82" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>360</v>
-      </c>
-      <c r="B83" s="1" t="s">
-        <v>441</v>
-      </c>
-      <c r="C83">
-        <v>5.9999879999999998E-2</v>
-      </c>
-      <c r="D83" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB0CFCFF-56D9-4568-B9DC-0986149CF27C}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -4369,7 +3304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26E65852-47FB-44B5-92C8-E9E1796557B8}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -4696,7 +3631,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3759851B-19B9-4E5B-9119-85C22D7372B5}">
   <dimension ref="A1:D37"/>
   <sheetViews>
@@ -5227,317 +4162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A462B9-8ADC-4100-81F1-D9D7D0B2E5A4}">
-  <dimension ref="A1:D21"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="18.7109375" customWidth="1"/>
-    <col min="2" max="2" width="38.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>442</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C2">
-        <v>0.94800296623867297</v>
-      </c>
-      <c r="D2" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>442</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>456</v>
-      </c>
-      <c r="C3">
-        <v>-298858410.89622402</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>442</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>457</v>
-      </c>
-      <c r="C4">
-        <v>1.2674442796410901</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>442</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>458</v>
-      </c>
-      <c r="C5">
-        <v>20.540277145606598</v>
-      </c>
-      <c r="D5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>442</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="C6">
-        <v>-3719998.2852976699</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>442</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>460</v>
-      </c>
-      <c r="C7">
-        <v>7591.3972498305102</v>
-      </c>
-      <c r="D7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>442</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>461</v>
-      </c>
-      <c r="C8">
-        <v>80.338319530249294</v>
-      </c>
-      <c r="D8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>442</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>462</v>
-      </c>
-      <c r="C9">
-        <v>2288.58796276767</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>442</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>463</v>
-      </c>
-      <c r="C10">
-        <v>0.91781499660108001</v>
-      </c>
-      <c r="D10" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>442</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C11">
-        <v>-83251849.276991397</v>
-      </c>
-      <c r="D11" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>442</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>466</v>
-      </c>
-      <c r="C12">
-        <v>169891.97606419999</v>
-      </c>
-      <c r="D12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>442</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>467</v>
-      </c>
-      <c r="C13">
-        <v>3.5898110791734701</v>
-      </c>
-      <c r="D13" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>442</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14">
-        <v>51217.545149546902</v>
-      </c>
-      <c r="D14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>442</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>468</v>
-      </c>
-      <c r="C15">
-        <v>22.3795396911936</v>
-      </c>
-      <c r="D15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>442</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>469</v>
-      </c>
-      <c r="C16">
-        <v>2658962.01212211</v>
-      </c>
-      <c r="D16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>442</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>470</v>
-      </c>
-      <c r="C17">
-        <v>367.553490500919</v>
-      </c>
-      <c r="D17" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>442</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>471</v>
-      </c>
-      <c r="C18">
-        <v>4.0441640741461997E-2</v>
-      </c>
-      <c r="D18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>442</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>472</v>
-      </c>
-      <c r="C19" s="3">
-        <v>1.39582181574593E-5</v>
-      </c>
-      <c r="D19" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>442</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>473</v>
-      </c>
-      <c r="C20" s="3">
-        <v>6.7955354538362796E-7</v>
-      </c>
-      <c r="D20" t="s">
-        <v>474</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>442</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>475</v>
-      </c>
-      <c r="C21">
-        <v>3.9112578160822502</v>
-      </c>
-      <c r="D21" t="s">
-        <v>31</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A95BED3-EF17-44FE-BB42-9D31FF6A18AC}">
   <dimension ref="A1:D34"/>
   <sheetViews>
@@ -6033,7 +4658,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95CC35DD-D2C1-4AD1-8561-DACD8B30634F}">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -6343,7 +4968,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DF2B6FE-9A2C-4C4A-A234-F0FC953692BB}">
   <dimension ref="A1:D22"/>
   <sheetViews>
@@ -6667,7 +5292,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{988AB2DB-E0BA-4FA9-BE3D-70423E0FABEA}">
   <dimension ref="A1:D36"/>
   <sheetViews>
@@ -7160,7 +5785,317 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95A462B9-8ADC-4100-81F1-D9D7D0B2E5A4}">
+  <dimension ref="A1:D21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" customWidth="1"/>
+    <col min="2" max="2" width="38.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>442</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>455</v>
+      </c>
+      <c r="C2">
+        <v>0.94800296623867297</v>
+      </c>
+      <c r="D2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="C3">
+        <v>-298858410.89622402</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>442</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>457</v>
+      </c>
+      <c r="C4">
+        <v>1.2674442796410901</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>442</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>458</v>
+      </c>
+      <c r="C5">
+        <v>20.540277145606598</v>
+      </c>
+      <c r="D5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>442</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>459</v>
+      </c>
+      <c r="C6">
+        <v>-3719998.2852976699</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>442</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>460</v>
+      </c>
+      <c r="C7">
+        <v>7591.3972498305102</v>
+      </c>
+      <c r="D7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>442</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>461</v>
+      </c>
+      <c r="C8">
+        <v>80.338319530249294</v>
+      </c>
+      <c r="D8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>442</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>462</v>
+      </c>
+      <c r="C9">
+        <v>2288.58796276767</v>
+      </c>
+      <c r="D9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>442</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>463</v>
+      </c>
+      <c r="C10">
+        <v>0.91781499660108001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>442</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C11">
+        <v>-83251849.276991397</v>
+      </c>
+      <c r="D11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>442</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>466</v>
+      </c>
+      <c r="C12">
+        <v>169891.97606419999</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>442</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>467</v>
+      </c>
+      <c r="C13">
+        <v>3.5898110791734701</v>
+      </c>
+      <c r="D13" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>442</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14">
+        <v>51217.545149546902</v>
+      </c>
+      <c r="D14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>442</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>468</v>
+      </c>
+      <c r="C15">
+        <v>22.3795396911936</v>
+      </c>
+      <c r="D15" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>442</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>469</v>
+      </c>
+      <c r="C16">
+        <v>2658962.01212211</v>
+      </c>
+      <c r="D16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>442</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="C17">
+        <v>367.553490500919</v>
+      </c>
+      <c r="D17" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>442</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>471</v>
+      </c>
+      <c r="C18">
+        <v>4.0441640741461997E-2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>442</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>472</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1.39582181574593E-5</v>
+      </c>
+      <c r="D19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>442</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>473</v>
+      </c>
+      <c r="C20" s="3">
+        <v>6.7955354538362796E-7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>442</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>475</v>
+      </c>
+      <c r="C21">
+        <v>3.9112578160822502</v>
+      </c>
+      <c r="D21" t="s">
+        <v>31</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5D025DD-F8B2-41BE-B6FB-E6B41E1A38EA}">
   <dimension ref="A1:D37"/>
   <sheetViews>
@@ -7675,661 +6610,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F3D0F3-EEDE-438A-B2DC-17A8742B4EBB}">
-  <dimension ref="A1:D47"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:D1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="22.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2">
-        <v>293.14999999999998</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C3">
-        <v>293.14999999999998</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="C4">
-        <v>123273.35425659201</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="C5">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6">
-        <v>408.60986664960001</v>
-      </c>
-      <c r="D6" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="C7">
-        <v>103.91882596765601</v>
-      </c>
-      <c r="D7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>59</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="C8">
-        <v>-71.000575536560603</v>
-      </c>
-      <c r="D8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9">
-        <v>50395977.811793096</v>
-      </c>
-      <c r="D9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C10">
-        <v>20.32</v>
-      </c>
-      <c r="D10" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>59</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="C11">
-        <v>0.1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="C13">
-        <v>0.3</v>
-      </c>
-      <c r="D13" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>59</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C14">
-        <v>3.3523173236731401</v>
-      </c>
-      <c r="D14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C15">
-        <v>1639.4002253300901</v>
-      </c>
-      <c r="D15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C16">
-        <v>1639.4002253300901</v>
-      </c>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>59</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C18">
-        <v>195998.70777802099</v>
-      </c>
-      <c r="D18" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>59</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C20">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C21">
-        <v>505.37222222222198</v>
-      </c>
-      <c r="D21" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>59</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="C22">
-        <v>0.19590411940819499</v>
-      </c>
-      <c r="D22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23">
-        <v>2637.89314990297</v>
-      </c>
-      <c r="D23" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C24">
-        <v>142.62426559289301</v>
-      </c>
-      <c r="D24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>59</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C25">
-        <v>8.5254842857698507E-2</v>
-      </c>
-      <c r="D25" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>59</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C26">
-        <v>4.2154916941611998E-4</v>
-      </c>
-      <c r="D26" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>59</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>92</v>
-      </c>
-      <c r="C27" s="1">
-        <v>3246.5053958447502</v>
-      </c>
-      <c r="D27" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>59</v>
-      </c>
-      <c r="B28" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="C28">
-        <v>3.1289602143091302E-2</v>
-      </c>
-      <c r="D28" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="C29" s="3">
-        <v>1.1115596804100299E-5</v>
-      </c>
-      <c r="D29" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>59</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="C30">
-        <v>142.62426559289301</v>
-      </c>
-      <c r="D30" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>59</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="C31">
-        <v>517106.93150815298</v>
-      </c>
-      <c r="D31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>59</v>
-      </c>
-      <c r="B32" s="1" t="s">
-        <v>97</v>
-      </c>
-      <c r="C32">
-        <v>616.48333333333301</v>
-      </c>
-      <c r="D32" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>59</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C33">
-        <v>3239.7983257679002</v>
-      </c>
-      <c r="D33" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>59</v>
-      </c>
-      <c r="B34" s="1" t="s">
-        <v>99</v>
-      </c>
-      <c r="C34">
-        <v>114.343194276283</v>
-      </c>
-      <c r="D34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C35">
-        <v>8.4150493001514295E-2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B36" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C36">
-        <v>1.9585300490304299E-4</v>
-      </c>
-      <c r="D36" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>59</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C37">
-        <v>3380.5862704330898</v>
-      </c>
-      <c r="D37" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>59</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C38">
-        <v>28.281071316610301</v>
-      </c>
-      <c r="D38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>59</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C39">
-        <v>3.6579554202880303E-2</v>
-      </c>
-      <c r="D39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>59</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="C40">
-        <v>507106.93150815298</v>
-      </c>
-      <c r="D40" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>59</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C41">
-        <v>0</v>
-      </c>
-      <c r="D41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>59</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42">
-        <v>987.84818533133205</v>
-      </c>
-      <c r="D42" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>59</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>59</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>110</v>
-      </c>
-      <c r="C44">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>59</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="C45" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>59</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="C46">
-        <v>0.4572</v>
-      </c>
-      <c r="D46" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>59</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C47">
-        <v>167732464.72469401</v>
-      </c>
-      <c r="D47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81E82467-585A-4152-BD71-4F59E74810DF}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -8672,12 +6953,666 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30F3D0F3-EEDE-438A-B2DC-17A8742B4EBB}">
+  <dimension ref="A1:D47"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.28515625" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2">
+        <v>293.14999999999998</v>
+      </c>
+      <c r="D2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3">
+        <v>293.14999999999998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4">
+        <v>123273.35425659201</v>
+      </c>
+      <c r="D4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C6">
+        <v>408.60986664960001</v>
+      </c>
+      <c r="D6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>59</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7">
+        <v>103.91882596765601</v>
+      </c>
+      <c r="D7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>59</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C8">
+        <v>-71.000575536560603</v>
+      </c>
+      <c r="D8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9">
+        <v>50395977.811793096</v>
+      </c>
+      <c r="D9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10">
+        <v>20.32</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>59</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C11">
+        <v>0.1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>59</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13">
+        <v>0.3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>59</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14">
+        <v>3.3523173236731401</v>
+      </c>
+      <c r="D14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>59</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C15">
+        <v>1639.4002253300901</v>
+      </c>
+      <c r="D15" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16">
+        <v>1639.4002253300901</v>
+      </c>
+      <c r="D16" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>59</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>59</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18">
+        <v>195998.70777802099</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>59</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C21">
+        <v>505.37222222222198</v>
+      </c>
+      <c r="D21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>59</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22">
+        <v>0.19590411940819499</v>
+      </c>
+      <c r="D22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>59</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23">
+        <v>2637.89314990297</v>
+      </c>
+      <c r="D23" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>59</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C24">
+        <v>142.62426559289301</v>
+      </c>
+      <c r="D24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>59</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C25">
+        <v>8.5254842857698507E-2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>59</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C26">
+        <v>4.2154916941611998E-4</v>
+      </c>
+      <c r="D26" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>59</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C27" s="1">
+        <v>3246.5053958447502</v>
+      </c>
+      <c r="D27" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>59</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28">
+        <v>3.1289602143091302E-2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>59</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1.1115596804100299E-5</v>
+      </c>
+      <c r="D29" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C30">
+        <v>142.62426559289301</v>
+      </c>
+      <c r="D30" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>59</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C31">
+        <v>517106.93150815298</v>
+      </c>
+      <c r="D31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C32">
+        <v>616.48333333333301</v>
+      </c>
+      <c r="D32" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C33">
+        <v>3239.7983257679002</v>
+      </c>
+      <c r="D33" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34">
+        <v>114.343194276283</v>
+      </c>
+      <c r="D34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>59</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C35">
+        <v>8.4150493001514295E-2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C36">
+        <v>1.9585300490304299E-4</v>
+      </c>
+      <c r="D36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>59</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C37">
+        <v>3380.5862704330898</v>
+      </c>
+      <c r="D37" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C38">
+        <v>28.281071316610301</v>
+      </c>
+      <c r="D38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>59</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C39">
+        <v>3.6579554202880303E-2</v>
+      </c>
+      <c r="D39" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>59</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C40">
+        <v>507106.93150815298</v>
+      </c>
+      <c r="D40" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>59</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>59</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42">
+        <v>987.84818533133205</v>
+      </c>
+      <c r="D42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>59</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>59</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="C45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>59</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C46">
+        <v>0.4572</v>
+      </c>
+      <c r="D46" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>59</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C47">
+        <v>167732464.72469401</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{421CE2E7-FC68-450D-806C-95F2AFE851FB}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="N33" sqref="N33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8733,7 +7668,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7001CFD8-AA2A-4C9C-A55B-353479567A7E}">
   <dimension ref="A1:D111"/>
   <sheetViews>
@@ -10308,7 +9243,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2565B27-3066-409B-84C5-A0659843152E}">
   <dimension ref="A1:D146"/>
   <sheetViews>
@@ -12373,7 +11308,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15FD9FF7-0411-4248-9C8B-0720113EB5E8}">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -12680,7 +11615,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61820C87-2A55-4B08-9C09-558D3CF708C4}">
   <dimension ref="A1:D24"/>
   <sheetViews>
@@ -13021,7 +11956,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC02C830-F897-4B2D-B23E-B55AD8B83A80}">
   <dimension ref="A1:D42"/>
   <sheetViews>
@@ -13614,7 +12549,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539FC3B6-C640-46D0-B9A7-855A0F3CAC49}">
   <dimension ref="A1:D48"/>
   <sheetViews>
@@ -14285,4 +13220,1069 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFFDE4E1-59B7-4973-8CE1-C8EF435EF1EA}">
+  <dimension ref="A1:D83"/>
+  <sheetViews>
+    <sheetView topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="B57" sqref="B57"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.5703125" customWidth="1"/>
+    <col min="2" max="2" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="C2">
+        <v>2.3103881337999899</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C3">
+        <v>5.4722559999999998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>360</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C4">
+        <v>298.14999999999998</v>
+      </c>
+      <c r="D4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>360</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C5">
+        <v>475.92910262650202</v>
+      </c>
+      <c r="D5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>360</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C6">
+        <v>4.62077626759997</v>
+      </c>
+      <c r="D6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>360</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>360</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C8">
+        <v>5.4796446382057002</v>
+      </c>
+      <c r="D8" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>360</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>360</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C10">
+        <v>0.60960000000000003</v>
+      </c>
+      <c r="D10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>360</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>360</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C12">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>360</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C13">
+        <v>5.7149999999999999E-2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>360</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C14">
+        <v>2.7990799999999999E-4</v>
+      </c>
+      <c r="D14" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>360</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C15" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>360</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>360</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>360</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>360</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>379</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>360</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>360</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>360</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>360</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C23">
+        <v>987095.20799758995</v>
+      </c>
+      <c r="D23" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>360</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C24">
+        <v>274.77419665194498</v>
+      </c>
+      <c r="D24" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>360</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>360</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>360</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>360</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>360</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C29">
+        <v>0.1463294</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>360</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C30">
+        <v>0.1222502</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>360</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>360</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>360</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C33">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>360</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>394</v>
+      </c>
+      <c r="D34" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>360</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>396</v>
+      </c>
+      <c r="C35">
+        <v>128.72530222576</v>
+      </c>
+      <c r="D35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>360</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>397</v>
+      </c>
+      <c r="C36">
+        <v>655.58755669238701</v>
+      </c>
+      <c r="D36" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>360</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>398</v>
+      </c>
+      <c r="C37">
+        <v>655.58755669238701</v>
+      </c>
+      <c r="D37" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>360</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>399</v>
+      </c>
+      <c r="C38">
+        <v>27.907387108739801</v>
+      </c>
+      <c r="D38" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>360</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C39">
+        <v>2.600006</v>
+      </c>
+      <c r="D39" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>360</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>401</v>
+      </c>
+      <c r="C40">
+        <v>31.472630310058602</v>
+      </c>
+      <c r="D40" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>360</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>402</v>
+      </c>
+      <c r="D41" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>360</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>403</v>
+      </c>
+      <c r="D42" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>360</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>404</v>
+      </c>
+      <c r="D43" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>360</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>405</v>
+      </c>
+      <c r="D44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>360</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>406</v>
+      </c>
+      <c r="D45" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>360</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>407</v>
+      </c>
+      <c r="D46" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>360</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>408</v>
+      </c>
+      <c r="D47" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>360</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="D48" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>360</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C49">
+        <v>699.81666666666695</v>
+      </c>
+      <c r="D49" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>360</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C50">
+        <v>18.779133793301298</v>
+      </c>
+      <c r="D50" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>360</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C51">
+        <v>5.0399669378168896</v>
+      </c>
+      <c r="D51" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>360</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C52">
+        <v>3362.68548838072</v>
+      </c>
+      <c r="D52" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>360</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C53">
+        <v>8.2194160102302904E-2</v>
+      </c>
+      <c r="D53" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>360</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2.1559459677269801E-5</v>
+      </c>
+      <c r="D54" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>360</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="D55" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>360</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C56">
+        <v>30</v>
+      </c>
+      <c r="D56" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>360</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C57">
+        <v>2.000006</v>
+      </c>
+      <c r="D57" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>360</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>417</v>
+      </c>
+      <c r="C58">
+        <v>5.1960779999999998E-2</v>
+      </c>
+      <c r="D58" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>360</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>418</v>
+      </c>
+      <c r="C59" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>360</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="C60">
+        <v>1.6509999999999999E-3</v>
+      </c>
+      <c r="D60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>360</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="C61">
+        <v>2.5399999999999999E-2</v>
+      </c>
+      <c r="D61" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>360</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>422</v>
+      </c>
+      <c r="D62" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>360</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>423</v>
+      </c>
+      <c r="D63" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>360</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>424</v>
+      </c>
+      <c r="D64" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>360</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>425</v>
+      </c>
+      <c r="D65" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>360</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>426</v>
+      </c>
+      <c r="D66" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>360</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>427</v>
+      </c>
+      <c r="D67" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>360</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>428</v>
+      </c>
+      <c r="D68" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>360</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>429</v>
+      </c>
+      <c r="D69" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>360</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="C70">
+        <v>639.87495207500899</v>
+      </c>
+      <c r="D70" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>360</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>430</v>
+      </c>
+      <c r="C71">
+        <v>20.610095210760001</v>
+      </c>
+      <c r="D71" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>360</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="C72">
+        <v>5.0399669378168896</v>
+      </c>
+      <c r="D72" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>360</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>432</v>
+      </c>
+      <c r="C73">
+        <v>31.472630310058602</v>
+      </c>
+      <c r="D73" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>360</v>
+      </c>
+      <c r="B74" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="C74">
+        <v>3172.2168225098299</v>
+      </c>
+      <c r="D74" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>360</v>
+      </c>
+      <c r="B75" s="1" t="s">
+        <v>434</v>
+      </c>
+      <c r="C75">
+        <v>7.2597136537635498E-2</v>
+      </c>
+      <c r="D75" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>360</v>
+      </c>
+      <c r="B76" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="C76" s="3">
+        <v>2.0231390664874999E-5</v>
+      </c>
+      <c r="D76" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>360</v>
+      </c>
+      <c r="B77" s="1" t="s">
+        <v>436</v>
+      </c>
+      <c r="D77" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>360</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="C78">
+        <v>44473.795433876803</v>
+      </c>
+      <c r="D78" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>360</v>
+      </c>
+      <c r="B79" s="1" t="s">
+        <v>438</v>
+      </c>
+      <c r="C79">
+        <v>14698.051332810899</v>
+      </c>
+      <c r="D79" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>360</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>439</v>
+      </c>
+      <c r="C80">
+        <v>3447379.5433876798</v>
+      </c>
+      <c r="D80" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>360</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>440</v>
+      </c>
+      <c r="C81">
+        <v>379191.81346832501</v>
+      </c>
+      <c r="D81" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>360</v>
+      </c>
+      <c r="B82" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C82">
+        <v>5.0399669378168896</v>
+      </c>
+      <c r="D82" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>360</v>
+      </c>
+      <c r="B83" s="1" t="s">
+        <v>441</v>
+      </c>
+      <c r="C83">
+        <v>5.9999879999999998E-2</v>
+      </c>
+      <c r="D83" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>